<commit_message>
Updated 15-Feb and chkd
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 21.xlsx
+++ b/Fix/fix cur. 21.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>amt</t>
   </si>
@@ -73,9 +73,6 @@
     <t>24105000106795</t>
   </si>
   <si>
-    <t>32108628506</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>913040005788755</t>
   </si>
   <si>
-    <t>50300001644294</t>
-  </si>
-  <si>
     <t>500 EOM</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>1111500111468501</t>
   </si>
   <si>
-    <t>50300030601844</t>
-  </si>
-  <si>
     <t xml:space="preserve">24106000093949  </t>
   </si>
   <si>
@@ -158,9 +149,6 @@
   </si>
   <si>
     <t>34145934830</t>
-  </si>
-  <si>
-    <t>Redeemed</t>
   </si>
   <si>
     <t>kk</t>
@@ -281,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -403,22 +391,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -812,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U114"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -899,57 +871,56 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:21" s="50" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A3" s="45">
-        <v>10.75</v>
-      </c>
-      <c r="B3" s="45">
+    <row r="3" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="B3" s="8">
         <v>9.25</v>
       </c>
-      <c r="C3" s="45">
-        <v>1</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="45" t="s">
+      <c r="C3" s="8">
+        <v>555</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46">
-        <v>41636</v>
-      </c>
-      <c r="H3" s="46">
-        <v>42366</v>
-      </c>
-      <c r="I3" s="47">
-        <f>24188/3</f>
-        <v>8062.666666666667</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="13">
+        <v>41713</v>
+      </c>
+      <c r="H3" s="13">
+        <v>42268</v>
+      </c>
+      <c r="I3" s="16">
+        <v>3442</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
     </row>
     <row r="4" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="8">
-        <v>4.5</v>
+        <v>6.75</v>
       </c>
       <c r="B4" s="8">
         <v>9.25</v>
       </c>
       <c r="C4" s="8">
-        <v>555</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>6</v>
@@ -957,18 +928,18 @@
       <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="43"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="13">
-        <v>41713</v>
+        <v>41887</v>
       </c>
       <c r="H4" s="13">
-        <v>42268</v>
+        <v>42252</v>
       </c>
       <c r="I4" s="16">
-        <v>3442</v>
+        <v>5164</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="10"/>
@@ -982,125 +953,125 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
     </row>
-    <row r="5" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="8">
-        <v>6.75</v>
-      </c>
-      <c r="B5" s="8">
-        <v>9.25</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8" t="s">
+    <row r="5" spans="1:21" s="48" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A5" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="B5" s="43">
+        <v>9</v>
+      </c>
+      <c r="C5" s="43">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="13">
-        <v>41887</v>
-      </c>
-      <c r="H5" s="13">
-        <v>42252</v>
-      </c>
-      <c r="I5" s="16">
-        <v>5164</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-    </row>
-    <row r="6" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="37">
-        <v>1.5</v>
-      </c>
-      <c r="B6" s="37">
-        <v>9</v>
-      </c>
-      <c r="C6" s="37">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="37" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="45">
+        <v>41941</v>
+      </c>
+      <c r="H5" s="45">
+        <v>42941</v>
+      </c>
+      <c r="I5" s="25">
+        <v>1117</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="43"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+    </row>
+    <row r="6" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <f>SUM(A3:A5)</f>
+        <v>12.75</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="7"/>
+      <c r="K6" s="7">
+        <f>SUM(I3:I4)</f>
+        <v>8606</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" s="21" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A7" s="8">
+        <v>12.3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="42">
-        <v>41941</v>
-      </c>
-      <c r="H6" s="42">
-        <v>42941</v>
-      </c>
-      <c r="I6" s="38">
-        <v>1117</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="37"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-    </row>
-    <row r="7" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3">
-        <f>SUM(A3:A6)</f>
-        <v>23.5</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="7"/>
-      <c r="K7" s="7">
-        <f>SUM(I3:I5)</f>
-        <v>16668.666666666668</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" s="21" customFormat="1" ht="12.75" customHeight="1">
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="18">
+        <v>41304</v>
+      </c>
+      <c r="H7" s="18">
+        <v>42399</v>
+      </c>
+      <c r="I7" s="44">
+        <v>10215</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+    </row>
+    <row r="8" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A8" s="8">
-        <v>12.3</v>
+        <v>6.15</v>
       </c>
       <c r="B8" s="8">
-        <v>10.050000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="C8" s="8">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
@@ -1110,38 +1081,38 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="18">
-        <v>41304</v>
+        <v>41480</v>
       </c>
       <c r="H8" s="18">
-        <v>42399</v>
-      </c>
-      <c r="I8" s="44">
-        <v>10215</v>
+        <v>42210</v>
+      </c>
+      <c r="I8" s="16">
+        <v>4830</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
+        <v>27</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
     </row>
     <row r="9" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="8">
-        <v>6.15</v>
+        <v>4.25</v>
       </c>
       <c r="B9" s="8">
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="C9" s="8">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>6</v>
@@ -1151,16 +1122,16 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="18">
-        <v>41480</v>
+        <v>41776</v>
       </c>
       <c r="H9" s="18">
-        <v>42210</v>
+        <v>42141</v>
       </c>
       <c r="I9" s="16">
-        <v>4830</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>29</v>
+        <v>3425</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="10"/>
@@ -1176,13 +1147,13 @@
     </row>
     <row r="10" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A10" s="8">
-        <v>4.25</v>
+        <v>2.85</v>
       </c>
       <c r="B10" s="8">
-        <v>9.75</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C10" s="8">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>6</v>
@@ -1192,16 +1163,16 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="18">
-        <v>41776</v>
+        <v>41816</v>
       </c>
       <c r="H10" s="18">
-        <v>42141</v>
+        <v>42547</v>
       </c>
       <c r="I10" s="16">
-        <v>3425</v>
+        <v>2309</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10" s="10"/>
@@ -1215,104 +1186,104 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A11" s="8">
-        <v>2.85</v>
-      </c>
-      <c r="B11" s="8">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="C11" s="8">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
+    <row r="11" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <f>SUM(A7:A10)</f>
+        <v>25.550000000000004</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="7">
+        <f>SUM(I7:I10)</f>
+        <v>20779</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A12" s="8">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>9.6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="18">
-        <v>41816</v>
-      </c>
-      <c r="H11" s="18">
-        <v>42547</v>
-      </c>
-      <c r="I11" s="16">
-        <v>2309</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-    </row>
-    <row r="12" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
-        <f>SUM(A8:A11)</f>
-        <v>25.550000000000004</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="7">
-        <f>SUM(I8:I11)</f>
-        <v>20779</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
+      <c r="E12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="13">
+        <v>41675</v>
+      </c>
+      <c r="H12" s="13">
+        <v>42171</v>
+      </c>
+      <c r="I12" s="28">
+        <v>3175</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="8">
-        <v>4</v>
+        <v>12.5</v>
       </c>
       <c r="B13" s="8">
-        <v>9.6</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>38</v>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="13">
-        <v>41675</v>
+        <v>41741</v>
       </c>
       <c r="H13" s="13">
-        <v>42171</v>
-      </c>
-      <c r="I13" s="28">
-        <v>3175</v>
+        <v>42241</v>
+      </c>
+      <c r="I13" s="16">
+        <v>10125</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="10"/>
@@ -1328,32 +1299,32 @@
     </row>
     <row r="14" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="A14" s="8">
-        <v>12.5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="8">
-        <v>9.8000000000000007</v>
+        <v>9.6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="13">
-        <v>41741</v>
+        <v>41838</v>
       </c>
       <c r="H14" s="13">
-        <v>42241</v>
+        <v>42203</v>
       </c>
       <c r="I14" s="16">
-        <v>10125</v>
+        <v>3175</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="10"/>
@@ -1367,262 +1338,258 @@
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A15" s="8">
-        <v>4</v>
-      </c>
-      <c r="B15" s="8">
-        <v>9.6</v>
-      </c>
-      <c r="C15" s="3" t="s">
+    <row r="15" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <f>SUM(A12:A14)</f>
+        <v>20.5</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="7">
+        <f>SUM(I12:I14)</f>
+        <v>16475</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A16" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="B16" s="8">
+        <v>9.18</v>
+      </c>
+      <c r="C16" s="8">
         <v>24</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="13">
-        <v>41838</v>
-      </c>
-      <c r="H15" s="13">
-        <v>42203</v>
-      </c>
-      <c r="I15" s="16">
-        <v>3175</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-    </row>
-    <row r="16" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <f>SUM(A13:A15)</f>
-        <v>20.5</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="7">
-        <f>SUM(I13:I15)</f>
-        <v>16475</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="1:21" s="54" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A17" s="43">
-        <v>4.3</v>
-      </c>
-      <c r="B17" s="43">
-        <v>9.18</v>
-      </c>
-      <c r="C17" s="43">
+      <c r="E16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="13">
+        <v>41442</v>
+      </c>
+      <c r="H16" s="13">
+        <v>42172</v>
+      </c>
+      <c r="I16" s="16">
+        <v>1871</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+    </row>
+    <row r="17" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A17" s="8">
+        <v>3.55</v>
+      </c>
+      <c r="B17" s="8">
+        <v>9.43</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="13">
+        <v>41761</v>
+      </c>
+      <c r="H17" s="13">
+        <v>42127</v>
+      </c>
+      <c r="I17" s="28">
+        <v>2843</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+    </row>
+    <row r="18" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <f>SUM(A16:A17)</f>
+        <v>5.9499999999999993</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="7">
+        <f>SUM(I16:I17)</f>
+        <v>4714</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A19" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="B19" s="8">
+        <v>10</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="13">
+        <v>41637</v>
+      </c>
+      <c r="H19" s="13">
+        <v>42367</v>
+      </c>
+      <c r="I19" s="16">
+        <v>2000</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+    </row>
+    <row r="20" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A20" s="37">
+        <v>3.9</v>
+      </c>
+      <c r="B20" s="37">
+        <v>9.75</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="42">
+        <v>41405</v>
+      </c>
+      <c r="H20" s="42">
+        <v>42105</v>
+      </c>
+      <c r="I20" s="38">
+        <v>3169</v>
+      </c>
+      <c r="J20" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="K20" s="37"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+    </row>
+    <row r="21" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A21" s="3">
+        <v>3.45</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="51">
-        <v>41313</v>
-      </c>
-      <c r="H17" s="51">
-        <v>42043</v>
-      </c>
-      <c r="I17" s="25">
-        <v>3353</v>
-      </c>
-      <c r="J17" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="43"/>
-      <c r="L17" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-    </row>
-    <row r="18" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A18" s="8">
-        <v>2.4</v>
-      </c>
-      <c r="B18" s="8">
-        <v>9.18</v>
-      </c>
-      <c r="C18" s="8">
-        <v>24</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="13">
-        <v>41442</v>
-      </c>
-      <c r="H18" s="13">
-        <v>42172</v>
-      </c>
-      <c r="I18" s="16">
-        <v>1871</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-    </row>
-    <row r="19" spans="1:21" s="54" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A19" s="43">
-        <v>11.9</v>
-      </c>
-      <c r="B19" s="43">
-        <v>9.43</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="51">
-        <v>41673</v>
-      </c>
-      <c r="H19" s="51">
-        <v>42039</v>
-      </c>
-      <c r="I19" s="25">
-        <v>9531</v>
-      </c>
-      <c r="J19" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-    </row>
-    <row r="20" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A20" s="8">
-        <v>3.55</v>
-      </c>
-      <c r="B20" s="8">
-        <v>9.43</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="13">
-        <v>41761</v>
-      </c>
-      <c r="H20" s="13">
-        <v>42127</v>
-      </c>
-      <c r="I20" s="28">
-        <v>2843</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-    </row>
-    <row r="21" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3">
-        <f>SUM(A17:A20)</f>
-        <v>22.150000000000002</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="7">
-        <f>SUM(I17:I20)</f>
-        <v>17598</v>
-      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="5">
+        <v>41429</v>
+      </c>
+      <c r="H21" s="5">
+        <v>42159</v>
+      </c>
+      <c r="I21" s="16">
+        <v>2803</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="3"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -1634,56 +1601,56 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
     </row>
-    <row r="22" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A22" s="8">
-        <v>2.4</v>
-      </c>
-      <c r="B22" s="8">
-        <v>10</v>
-      </c>
-      <c r="C22" s="8">
+    <row r="22" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A22" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="B22" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="C22" s="3">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="13">
-        <v>41637</v>
-      </c>
-      <c r="H22" s="13">
-        <v>42367</v>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5">
+        <v>41520</v>
+      </c>
+      <c r="H22" s="5">
+        <v>42250</v>
       </c>
       <c r="I22" s="16">
-        <v>2000</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-    </row>
-    <row r="23" spans="1:21" ht="12.75" customHeight="1">
+        <v>4672</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="1:21" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="A23" s="3">
-        <v>3.9</v>
+        <v>3.15</v>
       </c>
       <c r="B23" s="3">
         <v>9.75</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>25</v>
+      <c r="C23" s="3">
+        <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1693,32 +1660,32 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="5">
-        <v>41405</v>
+        <v>41536</v>
       </c>
       <c r="H23" s="5">
-        <v>42105</v>
+        <v>42266</v>
       </c>
       <c r="I23" s="16">
-        <v>3169</v>
+        <v>2559</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="K23" s="22"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
     </row>
     <row r="24" spans="1:21" ht="12.75" customHeight="1">
       <c r="A24" s="3">
-        <v>3.45</v>
+        <v>4.5</v>
       </c>
       <c r="B24" s="3">
         <v>9.75</v>
@@ -1734,16 +1701,16 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
-        <v>41429</v>
+        <v>41552</v>
       </c>
       <c r="H24" s="5">
-        <v>42159</v>
+        <v>42282</v>
       </c>
       <c r="I24" s="16">
-        <v>2803</v>
+        <v>3656</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
@@ -1757,118 +1724,89 @@
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
     </row>
-    <row r="25" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A25" s="3">
-        <v>5.75</v>
-      </c>
-      <c r="B25" s="3">
-        <v>9.75</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="3" t="s">
+    <row r="25" spans="1:21" s="34" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A25" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="B25" s="30">
+        <v>9</v>
+      </c>
+      <c r="C25" s="30">
+        <v>60</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="5">
-        <v>41520</v>
-      </c>
-      <c r="H25" s="5">
-        <v>42250</v>
-      </c>
-      <c r="I25" s="16">
-        <v>4672</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="1:21" s="24" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A26" s="3">
-        <v>3.15</v>
-      </c>
-      <c r="B26" s="3">
-        <v>9.75</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5">
-        <v>41536</v>
-      </c>
-      <c r="H26" s="5">
-        <v>42266</v>
-      </c>
-      <c r="I26" s="16">
-        <v>2559</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31">
+        <v>41650</v>
+      </c>
+      <c r="H25" s="31">
+        <v>43476</v>
+      </c>
+      <c r="I25" s="29">
+        <f>1125/3</f>
+        <v>375</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="30"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="33"/>
+    </row>
+    <row r="26" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <f>SUM(A19:A25)</f>
+        <v>23.65</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="7">
+        <f>SUM(I19:I24)</f>
+        <v>18859</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
     </row>
     <row r="27" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A27" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="B27" s="3">
-        <v>9.75</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="5">
-        <v>41552</v>
-      </c>
-      <c r="H27" s="5">
-        <v>42282</v>
-      </c>
-      <c r="I27" s="16">
-        <v>3656</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="7"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1880,66 +1818,77 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="1:21" s="34" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="B28" s="30">
-        <v>9</v>
-      </c>
-      <c r="C28" s="30">
-        <v>60</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31">
-        <v>41650</v>
-      </c>
-      <c r="H28" s="31">
-        <v>43476</v>
+    <row r="28" spans="1:21" s="53" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A28" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="B28" s="49">
+        <v>9.25</v>
+      </c>
+      <c r="C28" s="49">
+        <v>270</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="49"/>
+      <c r="G28" s="50">
+        <v>42010</v>
+      </c>
+      <c r="H28" s="50">
+        <v>42280</v>
       </c>
       <c r="I28" s="29">
-        <f>1125/3</f>
-        <v>375</v>
-      </c>
-      <c r="J28" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="30"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
+        <v>570</v>
+      </c>
+      <c r="J28" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="49"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
     </row>
     <row r="29" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3">
-        <f>SUM(A22:A28)</f>
-        <v>23.65</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="7">
-        <f>SUM(I22:I27)</f>
-        <v>18859</v>
-      </c>
+      <c r="A29" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="B29" s="3">
+        <v>9.18</v>
+      </c>
+      <c r="C29" s="3">
+        <v>270</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="5">
+        <v>42011</v>
+      </c>
+      <c r="H29" s="5">
+        <v>42281</v>
+      </c>
+      <c r="I29" s="16">
+        <v>2183</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" s="3"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -1952,17 +1901,35 @@
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="3">
+        <v>3.35</v>
+      </c>
+      <c r="B30" s="3">
+        <v>9.18</v>
+      </c>
+      <c r="C30" s="3">
+        <v>13</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="7"/>
+      <c r="G30" s="5">
+        <v>42012</v>
+      </c>
+      <c r="H30" s="5">
+        <v>42407</v>
+      </c>
+      <c r="I30" s="16">
+        <v>2612</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="3"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -1974,75 +1941,75 @@
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:21" s="59" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A31" s="55">
-        <v>0.25</v>
-      </c>
-      <c r="B31" s="55">
-        <v>9.25</v>
-      </c>
-      <c r="C31" s="55">
+    <row r="31" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A31" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="B31" s="3">
+        <v>9.18</v>
+      </c>
+      <c r="C31" s="3">
         <v>270</v>
       </c>
-      <c r="D31" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="55" t="s">
+      <c r="D31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="5">
+        <v>42017</v>
+      </c>
+      <c r="H31" s="5">
+        <v>42287</v>
+      </c>
+      <c r="I31" s="16">
+        <v>4210</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="55"/>
-      <c r="G31" s="56">
-        <v>42010</v>
-      </c>
-      <c r="H31" s="56">
-        <v>42280</v>
-      </c>
-      <c r="I31" s="29">
-        <v>570</v>
-      </c>
-      <c r="J31" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="55"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="58"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
     </row>
     <row r="32" spans="1:21" ht="12.75" customHeight="1">
       <c r="A32" s="3">
-        <v>2.8</v>
+        <v>5.4</v>
       </c>
       <c r="B32" s="3">
         <v>9.18</v>
       </c>
       <c r="C32" s="3">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="5">
-        <v>42011</v>
+        <v>42018</v>
       </c>
       <c r="H32" s="5">
-        <v>42281</v>
+        <v>42383</v>
       </c>
       <c r="I32" s="16">
-        <v>2183</v>
+        <v>4074</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="4"/>
@@ -2057,34 +2024,16 @@
       <c r="U32" s="4"/>
     </row>
     <row r="33" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A33" s="3">
-        <v>3.35</v>
-      </c>
-      <c r="B33" s="3">
-        <v>9.18</v>
-      </c>
-      <c r="C33" s="3">
-        <v>13</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="5">
-        <v>42012</v>
-      </c>
-      <c r="H33" s="5">
-        <v>42042</v>
-      </c>
-      <c r="I33" s="16">
-        <v>2612</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2098,34 +2047,19 @@
       <c r="U33" s="4"/>
     </row>
     <row r="34" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A34" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="B34" s="3">
-        <v>9.18</v>
-      </c>
-      <c r="C34" s="3">
-        <v>270</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5">
-        <v>42017</v>
-      </c>
-      <c r="H34" s="5">
-        <v>42287</v>
-      </c>
-      <c r="I34" s="16">
-        <v>4210</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <f>SUM(A28:A32)</f>
+        <v>17.200000000000003</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2139,34 +2073,16 @@
       <c r="U34" s="4"/>
     </row>
     <row r="35" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A35" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="B35" s="3">
-        <v>9.18</v>
-      </c>
-      <c r="C35" s="3">
-        <v>12</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="5">
-        <v>42018</v>
-      </c>
-      <c r="H35" s="5">
-        <v>42018</v>
-      </c>
-      <c r="I35" s="16">
-        <v>4074</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2185,11 +2101,15 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="7">
+        <f>SUM(I3:I32)</f>
+        <v>84574</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="K36" s="3"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2205,17 +2125,18 @@
     <row r="37" spans="1:21" ht="12.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3">
-        <f>SUM(A31:A35)</f>
-        <v>17.200000000000003</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="3"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="7">
+        <v>18095</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2230,14 +2151,13 @@
     </row>
     <row r="38" spans="1:21" ht="12.75" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="7"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="17"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
@@ -2254,19 +2174,19 @@
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="7">
-        <f>SUM(I3:I35)</f>
-        <v>105520.66666666667</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="1">
+        <f>SUM(F3:F34)</f>
+        <v>105.60000000000001</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="14">
+        <f>I36+I37</f>
+        <v>102669</v>
+      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2280,20 +2200,13 @@
       <c r="U39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="12"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="7">
-        <v>18095</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2307,14 +2220,12 @@
       <c r="U40" s="4"/>
     </row>
     <row r="41" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="11"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="17"/>
+      <c r="I41" s="4"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
@@ -2329,21 +2240,16 @@
       <c r="U41" s="4"/>
     </row>
     <row r="42" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42">
-        <v>400000</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="14">
-        <f>I39+I40</f>
-        <v>123615.66666666667</v>
-      </c>
-      <c r="J42" s="3"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="36"/>
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -2357,16 +2263,24 @@
       <c r="U42" s="4"/>
     </row>
     <row r="43" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="12"/>
-      <c r="G43">
-        <v>285000</v>
-      </c>
+      <c r="A43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C43" s="4">
+        <f>SUM(I19:I24) * 12 + 4*I25</f>
+        <v>227808</v>
+      </c>
+      <c r="E43" s="4">
+        <f>B43-C43</f>
+        <v>22192</v>
+      </c>
+      <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="36"/>
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2380,13 +2294,23 @@
       <c r="U43" s="4"/>
     </row>
     <row r="44" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="11"/>
-      <c r="E44" s="4"/>
+      <c r="A44" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C44" s="4">
+        <v>211176</v>
+      </c>
+      <c r="E44" s="4">
+        <f>B44-C44</f>
+        <v>38824</v>
+      </c>
+      <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="3"/>
+      <c r="J44" s="36"/>
       <c r="K44" s="3"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -2400,16 +2324,37 @@
       <c r="U44" s="4"/>
     </row>
     <row r="45" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C45" s="4">
+        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
+        <v>243076</v>
+      </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4">
+        <f t="shared" ref="E45:E47" si="0">B45-C45</f>
+        <v>6924</v>
+      </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="36"/>
+      <c r="G45">
+        <f>G39*0.1/12</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="17">
+        <v>9</v>
+      </c>
+      <c r="I45" s="17">
+        <f>G45*H45</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="35">
+        <f>C45+I45</f>
+        <v>243076</v>
+      </c>
       <c r="K45" s="3"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
@@ -2430,17 +2375,30 @@
         <v>250000</v>
       </c>
       <c r="C46" s="4">
-        <f>SUM(I22:I27) * 12 + 4*I28</f>
-        <v>227808</v>
-      </c>
+        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
+        <v>244803</v>
+      </c>
+      <c r="D46" s="4"/>
       <c r="E46" s="4">
         <f>B46-C46</f>
-        <v>22192</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="36"/>
+        <v>5197</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46">
+        <f>G40*0.1/12</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="17">
+        <v>9</v>
+      </c>
+      <c r="I46" s="17">
+        <f>G46*H46</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="35">
+        <f>C46+I46</f>
+        <v>244803</v>
+      </c>
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -2461,13 +2419,14 @@
         <v>250000</v>
       </c>
       <c r="C47" s="4">
-        <f>SUM(I17:I20) * 12</f>
-        <v>211176</v>
-      </c>
+        <v>174204</v>
+      </c>
+      <c r="D47" s="4"/>
       <c r="E47" s="4">
-        <f>B47-C47</f>
-        <v>38824</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>75796</v>
+      </c>
+      <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -2485,37 +2444,16 @@
       <c r="U47" s="4"/>
     </row>
     <row r="48" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A48" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C48" s="4">
-        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
-        <v>243076</v>
-      </c>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="4">
-        <f t="shared" ref="E48:E50" si="0">B48-C48</f>
-        <v>6924</v>
-      </c>
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48">
-        <f>G42*0.1/12</f>
-        <v>3333.3333333333335</v>
-      </c>
-      <c r="H48" s="17">
-        <v>9</v>
-      </c>
-      <c r="I48" s="17">
-        <f>G48*H48</f>
-        <v>30000</v>
-      </c>
-      <c r="J48" s="35">
-        <f>C48+I48</f>
-        <v>273076</v>
-      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -2529,37 +2467,16 @@
       <c r="U48" s="4"/>
     </row>
     <row r="49" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A49" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C49" s="4">
-        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
-        <v>244803</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="4">
-        <f>B49-C49</f>
-        <v>5197</v>
-      </c>
+      <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49">
-        <f>G43*0.1/12</f>
-        <v>2375</v>
-      </c>
-      <c r="H49" s="17">
-        <v>9</v>
-      </c>
-      <c r="I49" s="17">
-        <f>G49*H49</f>
-        <v>21375</v>
-      </c>
-      <c r="J49" s="35">
-        <f>C49+I49</f>
-        <v>266178</v>
-      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
@@ -2573,26 +2490,16 @@
       <c r="U49" s="4"/>
     </row>
     <row r="50" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C50" s="4">
-        <f>SUM(I3:I4) * 12 + I5 * 7</f>
-        <v>174204</v>
-      </c>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="4">
-        <f t="shared" si="0"/>
-        <v>75796</v>
-      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="36"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
@@ -2652,7 +2559,7 @@
       <c r="U52" s="4"/>
     </row>
     <row r="53" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A53" s="4"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2721,7 +2628,7 @@
       <c r="U55" s="4"/>
     </row>
     <row r="56" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A56" s="35"/>
+      <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -4008,75 +3915,6 @@
       <c r="T111" s="4"/>
       <c r="U111" s="4"/>
     </row>
-    <row r="112" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="3"/>
-      <c r="K112" s="3"/>
-      <c r="L112" s="4"/>
-      <c r="M112" s="4"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
-      <c r="Q112" s="4"/>
-      <c r="R112" s="4"/>
-      <c r="S112" s="4"/>
-      <c r="T112" s="4"/>
-      <c r="U112" s="4"/>
-    </row>
-    <row r="113" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="4"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
-      <c r="R113" s="4"/>
-      <c r="S113" s="4"/>
-      <c r="T113" s="4"/>
-      <c r="U113" s="4"/>
-    </row>
-    <row r="114" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="4"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
-      <c r="R114" s="4"/>
-      <c r="S114" s="4"/>
-      <c r="T114" s="4"/>
-      <c r="U114" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated 15-Feb hd new fd
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 21.xlsx
+++ b/Fix/fix cur. 21.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>amt</t>
   </si>
@@ -269,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -414,6 +414,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1449,161 +1452,161 @@
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
     </row>
-    <row r="18" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3">
-        <f>SUM(A16:A17)</f>
-        <v>5.9499999999999993</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="7">
+    <row r="18" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>9.18</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="13">
+        <v>42051</v>
+      </c>
+      <c r="H18" s="13">
+        <v>42782</v>
+      </c>
+      <c r="I18" s="25">
+        <v>13000</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <f>SUM(A16:A18)</f>
+        <v>22.95</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="7">
         <f>SUM(I16:I17)</f>
         <v>4714</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A19" s="8">
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="20" spans="1:21" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A20" s="8">
         <v>2.4</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B20" s="8">
         <v>10</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C20" s="8">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="13">
+      <c r="F20" s="8"/>
+      <c r="G20" s="13">
         <v>41637</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H20" s="13">
         <v>42367</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I20" s="16">
         <v>2000</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-    </row>
-    <row r="20" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A20" s="37">
+      <c r="K20" s="8"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+    </row>
+    <row r="21" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A21" s="37">
         <v>3.9</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B21" s="37">
         <v>9.75</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E21" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="42">
+      <c r="F21" s="37"/>
+      <c r="G21" s="42">
         <v>41405</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H21" s="42">
         <v>42105</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I21" s="38">
         <v>3169</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J21" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="37"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="40"/>
-      <c r="U20" s="40"/>
-    </row>
-    <row r="21" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A21" s="3">
-        <v>3.45</v>
-      </c>
-      <c r="B21" s="3">
-        <v>9.75</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="5">
-        <v>41429</v>
-      </c>
-      <c r="H21" s="5">
-        <v>42159</v>
-      </c>
-      <c r="I21" s="16">
-        <v>2803</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
     </row>
     <row r="22" spans="1:21" ht="12.75" customHeight="1">
       <c r="A22" s="3">
-        <v>5.75</v>
+        <v>3.45</v>
       </c>
       <c r="B22" s="3">
         <v>9.75</v>
@@ -1619,16 +1622,16 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="5">
-        <v>41520</v>
+        <v>41429</v>
       </c>
       <c r="H22" s="5">
-        <v>42250</v>
+        <v>42159</v>
       </c>
       <c r="I22" s="16">
-        <v>4672</v>
+        <v>2803</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="4"/>
@@ -1642,9 +1645,9 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
     </row>
-    <row r="23" spans="1:21" s="24" customFormat="1" ht="12.75" customHeight="1">
+    <row r="23" spans="1:21" ht="12.75" customHeight="1">
       <c r="A23" s="3">
-        <v>3.15</v>
+        <v>5.75</v>
       </c>
       <c r="B23" s="3">
         <v>9.75</v>
@@ -1660,32 +1663,32 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="5">
-        <v>41536</v>
+        <v>41520</v>
       </c>
       <c r="H23" s="5">
-        <v>42266</v>
+        <v>42250</v>
       </c>
       <c r="I23" s="16">
-        <v>2559</v>
+        <v>4672</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="22"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-    </row>
-    <row r="24" spans="1:21" ht="12.75" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="A24" s="3">
-        <v>4.5</v>
+        <v>3.15</v>
       </c>
       <c r="B24" s="3">
         <v>9.75</v>
@@ -1701,99 +1704,111 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
+        <v>41536</v>
+      </c>
+      <c r="H24" s="5">
+        <v>42266</v>
+      </c>
+      <c r="I24" s="16">
+        <v>2559</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" s="22"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+    </row>
+    <row r="25" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A25" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="B25" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="5">
         <v>41552</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H25" s="5">
         <v>42282</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I25" s="16">
         <v>3656</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="1:21" s="34" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A25" s="30">
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" s="34" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A26" s="30">
         <v>0.5</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B26" s="30">
         <v>9</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C26" s="30">
         <v>60</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D26" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E26" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31">
+      <c r="F26" s="30"/>
+      <c r="G26" s="31">
         <v>41650</v>
       </c>
-      <c r="H25" s="31">
+      <c r="H26" s="31">
         <v>43476</v>
       </c>
-      <c r="I25" s="29">
+      <c r="I26" s="29">
         <f>1125/3</f>
         <v>375</v>
       </c>
-      <c r="J25" s="32" t="s">
+      <c r="J26" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="30"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-    </row>
-    <row r="26" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3">
-        <f>SUM(A19:A25)</f>
-        <v>23.65</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="7">
-        <f>SUM(I19:I24)</f>
-        <v>18859</v>
-      </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
     </row>
     <row r="27" spans="1:21" ht="12.75" customHeight="1">
       <c r="A27" s="3"/>
@@ -1801,12 +1816,18 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3">
+        <f>SUM(A20:A26)</f>
+        <v>23.65</v>
+      </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="7"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="7"/>
+      <c r="K27" s="7">
+        <f>SUM(I20:I25)</f>
+        <v>18859</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1818,97 +1839,79 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="1:21" s="53" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="49">
+    <row r="28" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+    </row>
+    <row r="29" spans="1:21" s="53" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A29" s="49">
         <v>0.25</v>
       </c>
-      <c r="B28" s="49">
+      <c r="B29" s="49">
         <v>9.25</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C29" s="49">
         <v>270</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D29" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="49" t="s">
+      <c r="E29" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50">
+      <c r="F29" s="49"/>
+      <c r="G29" s="50">
         <v>42010</v>
       </c>
-      <c r="H28" s="50">
+      <c r="H29" s="50">
         <v>42280</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I29" s="29">
         <v>570</v>
       </c>
-      <c r="J28" s="51" t="s">
+      <c r="J29" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="49"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-    </row>
-    <row r="29" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A29" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="B29" s="3">
-        <v>9.18</v>
-      </c>
-      <c r="C29" s="3">
-        <v>270</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="5">
-        <v>42011</v>
-      </c>
-      <c r="H29" s="5">
-        <v>42281</v>
-      </c>
-      <c r="I29" s="16">
-        <v>2183</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="52"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="52"/>
     </row>
     <row r="30" spans="1:21" ht="12.75" customHeight="1">
       <c r="A30" s="3">
-        <v>3.35</v>
+        <v>2.8</v>
       </c>
       <c r="B30" s="3">
         <v>9.18</v>
       </c>
       <c r="C30" s="3">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>6</v>
@@ -1918,16 +1921,16 @@
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="5">
-        <v>42012</v>
+        <v>42011</v>
       </c>
       <c r="H30" s="5">
-        <v>42407</v>
+        <v>42281</v>
       </c>
       <c r="I30" s="16">
-        <v>2612</v>
+        <v>2183</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="4"/>
@@ -1943,13 +1946,13 @@
     </row>
     <row r="31" spans="1:21" ht="12.75" customHeight="1">
       <c r="A31" s="3">
-        <v>5.4</v>
+        <v>3.35</v>
       </c>
       <c r="B31" s="3">
         <v>9.18</v>
       </c>
       <c r="C31" s="3">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>6</v>
@@ -1959,16 +1962,16 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="5">
-        <v>42017</v>
+        <v>42012</v>
       </c>
       <c r="H31" s="5">
-        <v>42287</v>
+        <v>42407</v>
       </c>
       <c r="I31" s="16">
-        <v>4210</v>
+        <v>2612</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="4"/>
@@ -1990,7 +1993,7 @@
         <v>9.18</v>
       </c>
       <c r="C32" s="3">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
@@ -2000,16 +2003,16 @@
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="5">
-        <v>42018</v>
+        <v>42017</v>
       </c>
       <c r="H32" s="5">
-        <v>42383</v>
+        <v>42287</v>
       </c>
       <c r="I32" s="16">
-        <v>4074</v>
+        <v>4210</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="4"/>
@@ -2024,16 +2027,34 @@
       <c r="U32" s="4"/>
     </row>
     <row r="33" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="B33" s="3">
+        <v>9.18</v>
+      </c>
+      <c r="C33" s="3">
+        <v>12</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="3"/>
+      <c r="G33" s="5">
+        <v>42018</v>
+      </c>
+      <c r="H33" s="5">
+        <v>42383</v>
+      </c>
+      <c r="I33" s="16">
+        <v>4074</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2052,10 +2073,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3">
-        <f>SUM(A28:A32)</f>
-        <v>17.200000000000003</v>
-      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="7"/>
@@ -2078,7 +2096,10 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3">
+        <f>SUM(A29:A33)</f>
+        <v>17.200000000000003</v>
+      </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="7"/>
@@ -2101,15 +2122,11 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="7">
-        <f>SUM(I3:I32)</f>
-        <v>84574</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="I36" s="7"/>
+      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2125,17 +2142,17 @@
     <row r="37" spans="1:21" ht="12.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="7">
-        <v>18095</v>
+        <f>SUM(I3:I33)</f>
+        <v>97574</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="4"/>
@@ -2151,14 +2168,19 @@
     </row>
     <row r="38" spans="1:21" ht="12.75" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="7">
+        <v>18095</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2173,19 +2195,13 @@
     </row>
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="7"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="1">
-        <f>SUM(F3:F34)</f>
-        <v>105.60000000000001</v>
-      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="14">
-        <f>I36+I37</f>
-        <v>102669</v>
-      </c>
+      <c r="I39" s="17"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
@@ -2200,12 +2216,22 @@
       <c r="U39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="12"/>
+      <c r="A40" s="54">
+        <v>42050</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="1">
+        <f>SUM(F3:F35)</f>
+        <v>122.60000000000001</v>
+      </c>
       <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
+      <c r="I40" s="14">
+        <f>I37+I38</f>
+        <v>115669</v>
+      </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
@@ -2222,8 +2248,8 @@
     <row r="41" spans="1:21" ht="12.75" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="11"/>
-      <c r="E41" s="4"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="3"/>
@@ -2242,14 +2268,11 @@
     <row r="42" spans="1:21" ht="12.75" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="11"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="7"/>
+      <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="36"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -2263,22 +2286,14 @@
       <c r="U42" s="4"/>
     </row>
     <row r="43" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C43" s="4">
-        <f>SUM(I19:I24) * 12 + 4*I25</f>
-        <v>227808</v>
-      </c>
-      <c r="E43" s="4">
-        <f>B43-C43</f>
-        <v>22192</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="4"/>
       <c r="J43" s="36"/>
       <c r="K43" s="3"/>
@@ -2295,17 +2310,18 @@
     </row>
     <row r="44" spans="1:21" ht="12.75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="4">
         <v>250000</v>
       </c>
       <c r="C44" s="4">
-        <v>211176</v>
+        <f>SUM(I20:I25) * 12 + 4*I26</f>
+        <v>227808</v>
       </c>
       <c r="E44" s="4">
         <f>B44-C44</f>
-        <v>38824</v>
+        <v>22192</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2325,36 +2341,22 @@
     </row>
     <row r="45" spans="1:21" ht="12.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="4">
         <v>250000</v>
       </c>
       <c r="C45" s="4">
-        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
-        <v>243076</v>
-      </c>
-      <c r="D45" s="4"/>
+        <v>211176</v>
+      </c>
       <c r="E45" s="4">
-        <f t="shared" ref="E45:E47" si="0">B45-C45</f>
-        <v>6924</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45">
-        <f>G39*0.1/12</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="17">
-        <v>9</v>
-      </c>
-      <c r="I45" s="17">
-        <f>G45*H45</f>
-        <v>0</v>
-      </c>
-      <c r="J45" s="35">
-        <f>C45+I45</f>
-        <v>243076</v>
-      </c>
+        <f>B45-C45</f>
+        <v>38824</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="36"/>
       <c r="K45" s="3"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
@@ -2369,19 +2371,19 @@
     </row>
     <row r="46" spans="1:21" ht="12.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="4">
         <v>250000</v>
       </c>
       <c r="C46" s="4">
-        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
-        <v>244803</v>
+        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
+        <v>243076</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4">
-        <f>B46-C46</f>
-        <v>5197</v>
+        <f t="shared" ref="E46:E48" si="0">B46-C46</f>
+        <v>6924</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46">
@@ -2397,7 +2399,7 @@
       </c>
       <c r="J46" s="35">
         <f>C46+I46</f>
-        <v>244803</v>
+        <v>243076</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
@@ -2413,24 +2415,36 @@
     </row>
     <row r="47" spans="1:21" ht="12.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="4">
         <v>250000</v>
       </c>
       <c r="C47" s="4">
-        <v>174204</v>
+        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
+        <v>244803</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4">
-        <f t="shared" si="0"/>
-        <v>75796</v>
+        <f>B47-C47</f>
+        <v>5197</v>
       </c>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="36"/>
+      <c r="G47">
+        <f>G41*0.1/12</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="17">
+        <v>9</v>
+      </c>
+      <c r="I47" s="17">
+        <f>G47*H47</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="35">
+        <f>C47+I47</f>
+        <v>244803</v>
+      </c>
       <c r="K47" s="3"/>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
@@ -2444,16 +2458,25 @@
       <c r="U47" s="4"/>
     </row>
     <row r="48" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C48" s="4">
+        <v>174204</v>
+      </c>
       <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>75796</v>
+      </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="3"/>
+      <c r="J48" s="36"/>
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -2559,7 +2582,7 @@
       <c r="U52" s="4"/>
     </row>
     <row r="53" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A53" s="35"/>
+      <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2582,7 +2605,7 @@
       <c r="U53" s="4"/>
     </row>
     <row r="54" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A54" s="4"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -3915,6 +3938,29 @@
       <c r="T111" s="4"/>
       <c r="U111" s="4"/>
     </row>
+    <row r="112" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+      <c r="U112" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>